<commit_message>
Visual changes - 1
</commit_message>
<xml_diff>
--- a/DW+P5+-+Modele+plan+tests+acceptation.xlsx
+++ b/DW+P5+-+Modele+plan+tests+acceptation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Me/Documents/GitHub/Ouhabmehdi_5_25122021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48759B6-CACA-A143-A0B3-D169B19470B4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DC80D84-A635-DD45-9073-811362932CBC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -98,9 +98,6 @@
     <t>Affichage de l'ensemble des produits selectionnés par l'utilisateur ainsi qu'un formulaire d'envoi</t>
   </si>
   <si>
-    <t>Modification de la quantité et suppression d'article depuis la page panier</t>
-  </si>
-  <si>
     <t>Clique sur bouton "Supprimer" et clique sur champ modificateur de quantité</t>
   </si>
   <si>
@@ -141,6 +138,9 @@
   </si>
   <si>
     <t>Affichage d'un message de remerciement et numéro de commande unique correspondant à la commande passée par l'utilisateur</t>
+  </si>
+  <si>
+    <t>Modification de la quantité et suppression d'articles depuis la page panier</t>
   </si>
 </sst>
 </file>
@@ -648,7 +648,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -765,16 +765,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="10" t="s">
         <v>27</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="72" x14ac:dyDescent="0.15">
@@ -782,16 +782,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="D8" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="E8" s="10" t="s">
         <v>31</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="90" x14ac:dyDescent="0.15">
@@ -799,16 +799,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="D9" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="E9" s="10" t="s">
         <v>35</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="54" x14ac:dyDescent="0.15">
@@ -816,13 +816,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>38</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>39</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>10</v>

</xml_diff>